<commit_message>
116 paskaita - context ir reducer
</commit_message>
<xml_diff>
--- a/kalendorius.xlsx
+++ b/kalendorius.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Darbas\CodeAcademy\2022+\TypeScript7\praktika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB64255B-75BE-4036-8270-FD584FC3C05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CED2778-E473-4432-A773-4B8A822EBE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="C2:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>